<commit_message>
Fixed any running errors and can now reproduce result.
</commit_message>
<xml_diff>
--- a/results/FigureData1.xlsx
+++ b/results/FigureData1.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="55">
   <si>
     <t>doi</t>
   </si>
@@ -128,6 +129,57 @@
   </si>
   <si>
     <t>SUVmax</t>
+  </si>
+  <si>
+    <t>DataExtractionExample.png</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>Yields</t>
+  </si>
+  <si>
+    <t>(wt%)</t>
+  </si>
+  <si>
+    <t>50.0</t>
+  </si>
+  <si>
+    <t>40.0</t>
+  </si>
+  <si>
+    <t>30.0</t>
+  </si>
+  <si>
+    <t>20.0</t>
+  </si>
+  <si>
+    <t>10.0</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>Bio-oil</t>
+  </si>
+  <si>
+    <t>Solid</t>
+  </si>
+  <si>
+    <t>Gaseous product</t>
+  </si>
+  <si>
+    <t>Aqueous product</t>
   </si>
 </sst>
 </file>
@@ -206,6 +258,49 @@
         <a:xfrm>
           <a:off x="5486400" y="3810000"/>
           <a:ext cx="9020175" cy="7905750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>160351</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>68784</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="DataExtractionExample.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="3810000"/>
+          <a:ext cx="3817951" cy="2354784"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -805,4 +900,186 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10">
+        <v>7.8</v>
+      </c>
+      <c r="C10">
+        <v>14.7</v>
+      </c>
+      <c r="D10">
+        <v>15.1</v>
+      </c>
+      <c r="E10">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11">
+        <v>35.3</v>
+      </c>
+      <c r="C11">
+        <v>34.3</v>
+      </c>
+      <c r="D11">
+        <v>31</v>
+      </c>
+      <c r="E11">
+        <v>24.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12">
+        <v>16.5</v>
+      </c>
+      <c r="C12">
+        <v>19.8</v>
+      </c>
+      <c r="D12">
+        <v>19.6</v>
+      </c>
+      <c r="E12">
+        <v>22.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13">
+        <v>39.8</v>
+      </c>
+      <c r="C13">
+        <v>31</v>
+      </c>
+      <c r="D13">
+        <v>33.9</v>
+      </c>
+      <c r="E13">
+        <v>36.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>